<commit_message>
feat: correctly read multiple tables on one excel-sheet
</commit_message>
<xml_diff>
--- a/inst/extdata/example.xlsx
+++ b/inst/extdata/example.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="66">
   <si>
     <t xml:space="preserve">value_col</t>
   </si>
@@ -49,10 +49,25 @@
     <t xml:space="preserve">2025_col</t>
   </si>
   <si>
+    <t xml:space="preserve">2026_col</t>
+  </si>
+  <si>
     <t xml:space="preserve">Assets</t>
   </si>
   <si>
+    <t xml:space="preserve">test1_row</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test</t>
+  </si>
+  <si>
     <t xml:space="preserve">Fixed assets</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tes2_row</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Content</t>
   </si>
   <si>
     <t xml:space="preserve">int_fixed_assets_row</t>
@@ -487,10 +502,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D51"/>
+  <dimension ref="A1:J51"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
+      <selection pane="topLeft" activeCell="J8" activeCellId="0" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -542,28 +557,43 @@
       <c r="D6" s="1" t="s">
         <v>8</v>
       </c>
+      <c r="J6" s="0" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C7" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D7" s="3"/>
+      <c r="I7" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="J7" s="0" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C8" s="4" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="D8" s="5"/>
+      <c r="I8" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="J8" s="0" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="B9" s="1" t="n">
         <v>1</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="D9" s="5" t="n">
         <v>100000</v>
@@ -571,13 +601,13 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="B10" s="1" t="n">
         <v>2</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="D10" s="5" t="n">
         <v>200000</v>
@@ -585,13 +615,13 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="B11" s="1" t="n">
         <v>3</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="D11" s="5" t="n">
         <v>150000</v>
@@ -603,13 +633,13 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="B13" s="1" t="n">
         <v>4</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="D13" s="5" t="n">
         <f aca="false">SUM(D9:D11)</f>
@@ -622,19 +652,19 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C15" s="6" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="D15" s="5"/>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="B16" s="1" t="n">
         <v>5</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="D16" s="5" t="n">
         <v>25000</v>
@@ -642,13 +672,13 @@
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="B17" s="1" t="n">
         <v>6</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="D17" s="5" t="n">
         <v>15000</v>
@@ -656,13 +686,13 @@
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="B18" s="1" t="n">
         <v>7</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="D18" s="5" t="n">
         <v>10000</v>
@@ -670,13 +700,13 @@
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="B19" s="1" t="n">
         <v>8</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="D19" s="5" t="n">
         <v>400</v>
@@ -688,13 +718,13 @@
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="B21" s="1" t="n">
         <v>9</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="D21" s="5" t="n">
         <f aca="false">SUM(D16:D19)</f>
@@ -707,10 +737,10 @@
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="C23" s="6" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="D23" s="5" t="n">
         <f aca="false">SUM(E21+D13)</f>
@@ -723,25 +753,25 @@
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C25" s="4" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="D25" s="5"/>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C26" s="4" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="D26" s="5"/>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="B27" s="1" t="n">
         <v>10</v>
       </c>
       <c r="C27" s="6" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="D27" s="5" t="n">
         <v>75000</v>
@@ -749,13 +779,13 @@
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="B28" s="1" t="n">
         <v>11</v>
       </c>
       <c r="C28" s="6" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="D28" s="5" t="n">
         <v>25000</v>
@@ -763,13 +793,13 @@
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="B29" s="1" t="n">
         <v>12</v>
       </c>
       <c r="C29" s="6" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="D29" s="5" t="n">
         <v>10000</v>
@@ -781,13 +811,13 @@
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="1" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="B31" s="1" t="n">
         <v>13</v>
       </c>
       <c r="C31" s="6" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="D31" s="5" t="n">
         <f aca="false">SUM(D27:D29)</f>
@@ -800,13 +830,13 @@
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="1" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="B33" s="1" t="n">
         <v>14</v>
       </c>
       <c r="C33" s="6" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="D33" s="5" t="n">
         <v>20000</v>
@@ -818,19 +848,19 @@
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C35" s="4" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="D35" s="5"/>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="1" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="B36" s="1" t="n">
         <v>15</v>
       </c>
       <c r="C36" s="6" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="D36" s="5" t="n">
         <v>45000</v>
@@ -838,13 +868,13 @@
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="1" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="B37" s="1" t="n">
         <v>16</v>
       </c>
       <c r="C37" s="6" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="D37" s="5" t="n">
         <v>5000</v>
@@ -856,13 +886,13 @@
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="1" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="B39" s="1" t="n">
         <v>17</v>
       </c>
       <c r="C39" s="4" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="D39" s="5" t="n">
         <f aca="false">SUM(D36:D37)</f>
@@ -875,19 +905,19 @@
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C41" s="4" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="D41" s="5"/>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="1" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="B42" s="1" t="n">
         <v>18</v>
       </c>
       <c r="C42" s="6" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="D42" s="5" t="n">
         <v>20000</v>
@@ -899,13 +929,13 @@
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="1" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="B44" s="1" t="n">
         <v>19</v>
       </c>
       <c r="C44" s="6" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="D44" s="5" t="n">
         <f aca="false">D42</f>
@@ -918,19 +948,19 @@
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C46" s="4" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="D46" s="5"/>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="1" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="B47" s="1" t="n">
         <v>20</v>
       </c>
       <c r="C47" s="6" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="D47" s="5" t="n">
         <v>30000</v>
@@ -942,13 +972,13 @@
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="1" t="s">
-        <v>57</v>
+        <v>62</v>
       </c>
       <c r="B49" s="1" t="n">
         <v>21</v>
       </c>
       <c r="C49" s="6" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="D49" s="5" t="n">
         <f aca="false">D47</f>
@@ -961,13 +991,13 @@
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="1" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="B51" s="1" t="n">
         <v>22</v>
       </c>
       <c r="C51" s="7" t="s">
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="D51" s="8" t="n">
         <f aca="false">D31+D33+D39+D44+D48</f>

</xml_diff>